<commit_message>
Normalize all line endings
</commit_message>
<xml_diff>
--- a/examples/com.zeligsoft.domain.ngc.ccm.examples/ArtGallery/ArtGalleryImpInstCount.xlsx
+++ b/examples/com.zeligsoft.domain.ngc.ccm.examples/ArtGallery/ArtGalleryImpInstCount.xlsx
@@ -1,20 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="LocalityConstraint, Connection" sheetId="3" r:id="rId1"/>
-    <sheet name="Impl, Artifact, Instance" sheetId="1" r:id="rId2"/>
-    <sheet name="Properties" sheetId="4" r:id="rId3"/>
-    <sheet name="Rules" sheetId="2" r:id="rId4"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
-</file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="242">
@@ -7272,140 +7255,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
-    <col min="2" max="2" width="133.42578125" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="15">
-        <v>1</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="60">
-      <c r="A5" s="15">
-        <v>2</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="15">
-        <v>3</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30">
-      <c r="A7" s="15">
-        <v>4</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="15">
-        <v>5</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="15">
-        <v>6</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45">
-      <c r="A10" s="15">
-        <v>7</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="75">
-      <c r="A11" s="15">
-        <v>8</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>